<commit_message>
Correccion en archivo excel
</commit_message>
<xml_diff>
--- a/ActividadAlgoritmia1/EjeF(N).xlsx
+++ b/ActividadAlgoritmia1/EjeF(N).xlsx
@@ -9,14 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7800" firstSheet="3" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7800" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
-    <sheet name="Gráfico1" sheetId="5" r:id="rId4"/>
-    <sheet name="Hoja4" sheetId="4" r:id="rId5"/>
+    <sheet name="Hoja4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -177,6 +176,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -519,591 +519,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="es-CO"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Hoja4!$A$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>N</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:val>
-            <c:numRef>
-              <c:f>Hoja4!$A$2:$A$26</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="25"/>
-                <c:pt idx="0">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>120</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>140</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>160</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>180</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>200</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>220</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>240</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>260</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>280</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>300</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>320</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>340</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>360</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>380</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>400</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>420</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>440</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>460</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>480</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>500</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-9390-4481-A01A-209F054D446E}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Hoja4!$B$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>N Bytes</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:val>
-            <c:numRef>
-              <c:f>Hoja4!$B$2:$B$26</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="25"/>
-                <c:pt idx="0">
-                  <c:v>6592</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>25952</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>58112</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>103072</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>160832</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>231392</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>314752</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>410912</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>519872</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>641632</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>776192</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>923552</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1083712</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1256672</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1442432</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1640992</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1852352</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>2076512</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>2313472</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>2563232</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>2825792</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>3101152</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>3389312</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>3690272</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>4004032</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-9390-4481-A01A-209F054D446E}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Hoja4!$C$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>f(n)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:val>
-            <c:numRef>
-              <c:f>Hoja4!$C$2:$C$26</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="25"/>
-                <c:pt idx="0">
-                  <c:v>1226</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4846</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>10866</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>19286</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>30106</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>43326</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>58946</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>76966</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>97386</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>120206</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>145426</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>173046</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>203066</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>235486</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>270306</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>307526</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>347146</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>389166</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>433586</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>480406</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>529626</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>581246</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>635266</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>691686</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>750506</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-9390-4481-A01A-209F054D446E}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="2134814847"/>
-        <c:axId val="2134813183"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="2134814847"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="es-CO"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="2134813183"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="2134813183"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="es-CO"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="2134814847"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="es-CO"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="es-CO"/>
-    </a:p>
-  </c:txPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
       <c:tx>
         <c:rich>
           <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
@@ -1552,7 +967,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
@@ -2015,7 +1430,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
@@ -2682,6 +2097,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6372,46 +5788,6 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors13.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -7249,7 +6625,7 @@
 </file>
 
 <file path=xl/charts/style10.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -7276,8 +6652,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -7378,7 +6754,7 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+      <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -7410,10 +6786,10 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -7453,22 +6829,23 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -7573,8 +6950,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -7706,19 +7083,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -7732,6 +7110,17 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -8268,7 +7657,7 @@
 </file>
 
 <file path=xl/charts/style12.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -8295,8 +7684,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -8376,6 +7765,11 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -8386,6 +7780,11 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -8397,7 +7796,7 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="19050" cap="rnd">
+      <a:ln w="28575" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -8417,6 +7816,9 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -8429,10 +7831,10 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -8472,23 +7874,22 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -8593,8 +7994,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -8726,20 +8127,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -8753,17 +8153,6 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -8783,8 +8172,8 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style13.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -8811,8 +8200,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -8892,11 +8281,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -8907,11 +8291,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -8923,7 +8302,7 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+      <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -8943,9 +8322,6 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -8958,10 +8334,10 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -9001,22 +8377,23 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -9121,8 +8498,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -9254,19 +8631,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -9280,6 +8658,17 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -9299,8 +8688,8 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -9327,8 +8716,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -9408,6 +8797,11 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -9418,6 +8812,11 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -9429,7 +8828,7 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="19050" cap="rnd">
+      <a:ln w="28575" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -9449,6 +8848,9 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -9461,10 +8863,10 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -9504,23 +8906,22 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -9625,8 +9026,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -9758,20 +9159,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -9785,17 +9185,6 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -9815,8 +9204,8 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -9843,8 +9232,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -9924,11 +9313,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -9939,11 +9323,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -9955,7 +9334,7 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+      <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -9975,9 +9354,6 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -9990,10 +9366,10 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -10033,22 +9409,23 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -10153,8 +9530,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -10286,19 +9663,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -10312,6 +9690,17 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -10331,7 +9720,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -10847,8 +10236,8 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -10875,8 +10264,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -10956,6 +10345,11 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -10966,6 +10360,11 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -10977,7 +10376,7 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="19050" cap="rnd">
+      <a:ln w="28575" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -10997,6 +10396,9 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -11009,10 +10411,10 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -11052,23 +10454,22 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -11173,8 +10574,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -11306,20 +10707,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -11333,17 +10733,6 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -11363,8 +10752,8 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -11391,8 +10780,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -11472,11 +10861,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -11487,11 +10871,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -11503,7 +10882,7 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+      <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -11523,9 +10902,6 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -11538,10 +10914,10 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -11581,22 +10957,23 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -11701,8 +11078,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -11834,19 +11211,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -11860,6 +11238,17 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -11879,7 +11268,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -12395,8 +11784,8 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+<file path=xl/charts/style9.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -12423,8 +11812,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -12504,6 +11893,11 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -12514,6 +11908,11 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -12525,7 +11924,7 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="19050" cap="rnd">
+      <a:ln w="28575" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -12545,532 +11944,6 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style9.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="phClr"/>
       </a:solidFill>
@@ -13425,17 +12298,6 @@
     </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
-</file>
-
-<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr/>
-  <sheetViews>
-    <sheetView zoomScale="53" workbookViewId="0" zoomToFit="1"/>
-  </sheetViews>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</chartsheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -13755,33 +12617,6 @@
 
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:absoluteAnchor>
-    <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8662358" cy="6272123"/>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Gráfico 1"/>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks noGrp="1"/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:absoluteAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
@@ -14814,7 +13649,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:C26"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Creacion de algoritmo burbuja y mediciones del mismo
</commit_message>
<xml_diff>
--- a/ActividadAlgoritmia1/EjeF(N).xlsx
+++ b/ActividadAlgoritmia1/EjeF(N).xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20384"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Descargas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Camilo\Universidad\Sexto Semestre\Ciencias1\ActividadAlgoritmia1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4E8E252-C5DC-4306-A30C-1BD7893DDF14}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
     <sheet name="Hoja4" sheetId="4" r:id="rId4"/>
+    <sheet name="Burbuja" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="12">
   <si>
     <t>N</t>
   </si>
@@ -62,11 +62,26 @@
   <si>
     <t>t(microsgs)</t>
   </si>
+  <si>
+    <t>t(N)</t>
+  </si>
+  <si>
+    <t>tiempo(seg)</t>
+  </si>
+  <si>
+    <t>tiempo(microseg)</t>
+  </si>
+  <si>
+    <t>Peor</t>
+  </si>
+  <si>
+    <t>Mejor</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -138,7 +153,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -154,6 +169,13 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -242,7 +264,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -430,7 +452,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="285939344"/>
@@ -492,7 +514,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="292216592"/>
@@ -533,7 +555,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-US"/>
+      <a:endParaRPr lang="es-CO"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -614,7 +636,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -892,7 +914,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1631631007"/>
@@ -954,7 +976,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1498540687"/>
@@ -995,7 +1017,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-US"/>
+      <a:endParaRPr lang="es-CO"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1076,7 +1098,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1354,7 +1376,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2102543199"/>
@@ -1416,7 +1438,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2102539871"/>
@@ -1457,7 +1479,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-US"/>
+      <a:endParaRPr lang="es-CO"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1513,6 +1535,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1538,7 +1561,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1816,7 +1839,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2134812767"/>
@@ -1878,7 +1901,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2134821919"/>
@@ -1919,7 +1942,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-US"/>
+      <a:endParaRPr lang="es-CO"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1970,7 +1993,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2413,7 +2436,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2102538623"/>
@@ -2472,7 +2495,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2102546943"/>
@@ -2514,7 +2537,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2544,7 +2567,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-US"/>
+      <a:endParaRPr lang="es-CO"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2570,6 +2593,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2595,7 +2619,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2873,7 +2897,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1400550767"/>
@@ -2935,7 +2959,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1668870943"/>
@@ -2976,7 +3000,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-US"/>
+      <a:endParaRPr lang="es-CO"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3052,7 +3076,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3240,7 +3264,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="429262704"/>
@@ -3302,7 +3326,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="297415840"/>
@@ -3343,7 +3367,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-US"/>
+      <a:endParaRPr lang="es-CO"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3394,7 +3418,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3657,7 +3681,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="433823584"/>
@@ -3716,7 +3740,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="519424336"/>
@@ -3758,7 +3782,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3788,7 +3812,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-US"/>
+      <a:endParaRPr lang="es-CO"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3869,7 +3893,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -4057,7 +4081,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="427246960"/>
@@ -4119,7 +4143,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="512862000"/>
@@ -4160,7 +4184,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-US"/>
+      <a:endParaRPr lang="es-CO"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -4236,7 +4260,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -4424,7 +4448,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="523413248"/>
@@ -4486,7 +4510,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="513921296"/>
@@ -4527,7 +4551,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-US"/>
+      <a:endParaRPr lang="es-CO"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -4578,7 +4602,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -4841,7 +4865,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2048971615"/>
@@ -4900,7 +4924,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2048969535"/>
@@ -4942,7 +4966,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -4972,7 +4996,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-US"/>
+      <a:endParaRPr lang="es-CO"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -5053,7 +5077,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -5331,7 +5355,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2128402687"/>
@@ -5393,7 +5417,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2128402271"/>
@@ -5434,7 +5458,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-US"/>
+      <a:endParaRPr lang="es-CO"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -5510,7 +5534,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -5788,7 +5812,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2134810271"/>
@@ -5850,7 +5874,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2134811519"/>
@@ -5891,7 +5915,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-US"/>
+      <a:endParaRPr lang="es-CO"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -5942,7 +5966,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -6407,7 +6431,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2006456879"/>
@@ -6466,7 +6490,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2128404351"/>
@@ -6508,7 +6532,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -6538,7 +6562,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-US"/>
+      <a:endParaRPr lang="es-CO"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -15153,7 +15177,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -15310,7 +15334,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
@@ -15466,7 +15490,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C64"/>
   <sheetViews>
     <sheetView topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
@@ -16108,10 +16132,10 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A26" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>
@@ -16743,4 +16767,1567 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I52"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:I1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" style="6"/>
+    <col min="4" max="4" width="16.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="F1" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="6">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <f>(A3^2-A3)/2</f>
+        <v>45</v>
+      </c>
+      <c r="C3" s="6">
+        <v>3.0000000000000001E-6</v>
+      </c>
+      <c r="D3">
+        <f>C3*1000000</f>
+        <v>3</v>
+      </c>
+      <c r="F3" s="6">
+        <v>10</v>
+      </c>
+      <c r="G3">
+        <f>F3^2-F3</f>
+        <v>90</v>
+      </c>
+      <c r="H3" s="6">
+        <v>3.9999999999999998E-6</v>
+      </c>
+      <c r="I3">
+        <f>H3*1000000</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="6">
+        <v>20</v>
+      </c>
+      <c r="B4">
+        <f t="shared" ref="B4:B52" si="0">(A4^2-A4)/2</f>
+        <v>190</v>
+      </c>
+      <c r="C4" s="6">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="D4">
+        <f t="shared" ref="D4:D52" si="1">C4*1000000</f>
+        <v>2</v>
+      </c>
+      <c r="F4" s="6">
+        <v>20</v>
+      </c>
+      <c r="G4">
+        <f t="shared" ref="G4:G52" si="2">F4^2-F4</f>
+        <v>380</v>
+      </c>
+      <c r="H4" s="6">
+        <v>3.0000000000000001E-6</v>
+      </c>
+      <c r="I4">
+        <f t="shared" ref="I4:I52" si="3">H4*1000000</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="6">
+        <v>30</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="0"/>
+        <v>435</v>
+      </c>
+      <c r="C5" s="6">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F5" s="6">
+        <v>30</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="2"/>
+        <v>870</v>
+      </c>
+      <c r="H5" s="6">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="6">
+        <v>40</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>780</v>
+      </c>
+      <c r="C6" s="6">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F6" s="6">
+        <v>40</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="2"/>
+        <v>1560</v>
+      </c>
+      <c r="H6" s="6">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="6">
+        <v>50</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>1225</v>
+      </c>
+      <c r="C7" s="6">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="F7" s="6">
+        <v>50</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="2"/>
+        <v>2450</v>
+      </c>
+      <c r="H7" s="6">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="6">
+        <v>60</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>1770</v>
+      </c>
+      <c r="C8" s="6">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F8" s="6">
+        <v>60</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="2"/>
+        <v>3540</v>
+      </c>
+      <c r="H8" s="6">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="6">
+        <v>70</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>2415</v>
+      </c>
+      <c r="C9" s="6">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F9" s="6">
+        <v>70</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="2"/>
+        <v>4830</v>
+      </c>
+      <c r="H9" s="6">
+        <v>3.0000000000000001E-6</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="6">
+        <v>80</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>3160</v>
+      </c>
+      <c r="C10" s="6">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F10" s="6">
+        <v>80</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="2"/>
+        <v>6320</v>
+      </c>
+      <c r="H10" s="6">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="6">
+        <v>90</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>4005</v>
+      </c>
+      <c r="C11" s="6">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F11" s="6">
+        <v>90</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="2"/>
+        <v>8010</v>
+      </c>
+      <c r="H11" s="6">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="6">
+        <v>100</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="0"/>
+        <v>4950</v>
+      </c>
+      <c r="C12" s="6">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F12" s="6">
+        <v>100</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="2"/>
+        <v>9900</v>
+      </c>
+      <c r="H12" s="6">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="6">
+        <v>110</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="0"/>
+        <v>5995</v>
+      </c>
+      <c r="C13" s="6">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F13" s="6">
+        <v>110</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="2"/>
+        <v>11990</v>
+      </c>
+      <c r="H13" s="6">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="6">
+        <v>120</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="0"/>
+        <v>7140</v>
+      </c>
+      <c r="C14" s="6">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F14" s="6">
+        <v>120</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="2"/>
+        <v>14280</v>
+      </c>
+      <c r="H14" s="6">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="6">
+        <v>130</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="0"/>
+        <v>8385</v>
+      </c>
+      <c r="C15" s="6">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F15" s="6">
+        <v>130</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="2"/>
+        <v>16770</v>
+      </c>
+      <c r="H15" s="6">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="6">
+        <v>140</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>9730</v>
+      </c>
+      <c r="C16" s="6">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F16" s="6">
+        <v>140</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="2"/>
+        <v>19460</v>
+      </c>
+      <c r="H16" s="6">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="6">
+        <v>150</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>11175</v>
+      </c>
+      <c r="C17" s="6">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="F17" s="6">
+        <v>150</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="2"/>
+        <v>22350</v>
+      </c>
+      <c r="H17" s="6">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="6">
+        <v>160</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="0"/>
+        <v>12720</v>
+      </c>
+      <c r="C18" s="6">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F18" s="6">
+        <v>160</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="2"/>
+        <v>25440</v>
+      </c>
+      <c r="H18" s="6">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="6">
+        <v>170</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="0"/>
+        <v>14365</v>
+      </c>
+      <c r="C19" s="6">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="F19" s="6">
+        <v>170</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="2"/>
+        <v>28730</v>
+      </c>
+      <c r="H19" s="6">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="6">
+        <v>180</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="0"/>
+        <v>16110</v>
+      </c>
+      <c r="C20" s="6">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F20" s="6">
+        <v>180</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="2"/>
+        <v>32220</v>
+      </c>
+      <c r="H20" s="6">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="6">
+        <v>190</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="0"/>
+        <v>17955</v>
+      </c>
+      <c r="C21" s="6">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F21" s="6">
+        <v>190</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="2"/>
+        <v>35910</v>
+      </c>
+      <c r="H21" s="6">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="6">
+        <v>200</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="0"/>
+        <v>19900</v>
+      </c>
+      <c r="C22" s="6">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F22" s="6">
+        <v>200</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="2"/>
+        <v>39800</v>
+      </c>
+      <c r="H22" s="6">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="6">
+        <v>210</v>
+      </c>
+      <c r="B23">
+        <f t="shared" si="0"/>
+        <v>21945</v>
+      </c>
+      <c r="C23" s="6">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F23" s="6">
+        <v>210</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="2"/>
+        <v>43890</v>
+      </c>
+      <c r="H23" s="6">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="6">
+        <v>220</v>
+      </c>
+      <c r="B24">
+        <f t="shared" si="0"/>
+        <v>24090</v>
+      </c>
+      <c r="C24" s="6">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F24" s="6">
+        <v>220</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="2"/>
+        <v>48180</v>
+      </c>
+      <c r="H24" s="6">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="6">
+        <v>230</v>
+      </c>
+      <c r="B25">
+        <f t="shared" si="0"/>
+        <v>26335</v>
+      </c>
+      <c r="C25" s="6">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F25" s="6">
+        <v>230</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="2"/>
+        <v>52670</v>
+      </c>
+      <c r="H25" s="6">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="6">
+        <v>240</v>
+      </c>
+      <c r="B26">
+        <f t="shared" si="0"/>
+        <v>28680</v>
+      </c>
+      <c r="C26" s="6">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F26" s="6">
+        <v>240</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="2"/>
+        <v>57360</v>
+      </c>
+      <c r="H26" s="6">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="6">
+        <v>250</v>
+      </c>
+      <c r="B27">
+        <f t="shared" si="0"/>
+        <v>31125</v>
+      </c>
+      <c r="C27" s="6">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F27" s="6">
+        <v>250</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="2"/>
+        <v>62250</v>
+      </c>
+      <c r="H27" s="6">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="6">
+        <v>260</v>
+      </c>
+      <c r="B28">
+        <f t="shared" si="0"/>
+        <v>33670</v>
+      </c>
+      <c r="C28" s="6">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F28" s="6">
+        <v>260</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="2"/>
+        <v>67340</v>
+      </c>
+      <c r="H28" s="6">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="6">
+        <v>270</v>
+      </c>
+      <c r="B29">
+        <f t="shared" si="0"/>
+        <v>36315</v>
+      </c>
+      <c r="C29" s="6">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F29" s="6">
+        <v>270</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="2"/>
+        <v>72630</v>
+      </c>
+      <c r="H29" s="6">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="6">
+        <v>280</v>
+      </c>
+      <c r="B30">
+        <f t="shared" si="0"/>
+        <v>39060</v>
+      </c>
+      <c r="C30" s="6">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F30" s="6">
+        <v>280</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="2"/>
+        <v>78120</v>
+      </c>
+      <c r="H30" s="6">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="6">
+        <v>290</v>
+      </c>
+      <c r="B31">
+        <f t="shared" si="0"/>
+        <v>41905</v>
+      </c>
+      <c r="C31" s="6">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F31" s="6">
+        <v>290</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="2"/>
+        <v>83810</v>
+      </c>
+      <c r="H31" s="6">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="I31">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="6">
+        <v>300</v>
+      </c>
+      <c r="B32">
+        <f t="shared" si="0"/>
+        <v>44850</v>
+      </c>
+      <c r="C32" s="6">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="F32" s="6">
+        <v>300</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="2"/>
+        <v>89700</v>
+      </c>
+      <c r="H32" s="6">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="I32">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="6">
+        <v>310</v>
+      </c>
+      <c r="B33">
+        <f t="shared" si="0"/>
+        <v>47895</v>
+      </c>
+      <c r="C33" s="6">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="F33" s="6">
+        <v>310</v>
+      </c>
+      <c r="G33">
+        <f t="shared" si="2"/>
+        <v>95790</v>
+      </c>
+      <c r="H33" s="6">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="I33">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="6">
+        <v>320</v>
+      </c>
+      <c r="B34">
+        <f t="shared" si="0"/>
+        <v>51040</v>
+      </c>
+      <c r="C34" s="6">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F34" s="6">
+        <v>320</v>
+      </c>
+      <c r="G34">
+        <f t="shared" si="2"/>
+        <v>102080</v>
+      </c>
+      <c r="H34" s="6">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="I34">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="6">
+        <v>330</v>
+      </c>
+      <c r="B35">
+        <f t="shared" si="0"/>
+        <v>54285</v>
+      </c>
+      <c r="C35" s="6">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F35" s="6">
+        <v>330</v>
+      </c>
+      <c r="G35">
+        <f t="shared" si="2"/>
+        <v>108570</v>
+      </c>
+      <c r="H35" s="6">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="I35">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="6">
+        <v>340</v>
+      </c>
+      <c r="B36">
+        <f t="shared" si="0"/>
+        <v>57630</v>
+      </c>
+      <c r="C36" s="6">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F36" s="6">
+        <v>340</v>
+      </c>
+      <c r="G36">
+        <f t="shared" si="2"/>
+        <v>115260</v>
+      </c>
+      <c r="H36" s="6">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="I36">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="6">
+        <v>350</v>
+      </c>
+      <c r="B37">
+        <f t="shared" si="0"/>
+        <v>61075</v>
+      </c>
+      <c r="C37" s="6">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="D37">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F37" s="6">
+        <v>350</v>
+      </c>
+      <c r="G37">
+        <f t="shared" si="2"/>
+        <v>122150</v>
+      </c>
+      <c r="H37" s="6">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="I37">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="6">
+        <v>360</v>
+      </c>
+      <c r="B38">
+        <f t="shared" si="0"/>
+        <v>64620</v>
+      </c>
+      <c r="C38" s="6">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F38" s="6">
+        <v>360</v>
+      </c>
+      <c r="G38">
+        <f t="shared" si="2"/>
+        <v>129240</v>
+      </c>
+      <c r="H38" s="6">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="I38">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="6">
+        <v>370</v>
+      </c>
+      <c r="B39">
+        <f t="shared" si="0"/>
+        <v>68265</v>
+      </c>
+      <c r="C39" s="6">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="D39">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F39" s="6">
+        <v>370</v>
+      </c>
+      <c r="G39">
+        <f t="shared" si="2"/>
+        <v>136530</v>
+      </c>
+      <c r="H39" s="6">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="I39">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="6">
+        <v>380</v>
+      </c>
+      <c r="B40">
+        <f t="shared" si="0"/>
+        <v>72010</v>
+      </c>
+      <c r="C40" s="6">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="D40">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F40" s="6">
+        <v>380</v>
+      </c>
+      <c r="G40">
+        <f t="shared" si="2"/>
+        <v>144020</v>
+      </c>
+      <c r="H40" s="6">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="I40">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="6">
+        <v>390</v>
+      </c>
+      <c r="B41">
+        <f t="shared" si="0"/>
+        <v>75855</v>
+      </c>
+      <c r="C41" s="6">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="D41">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="F41" s="6">
+        <v>390</v>
+      </c>
+      <c r="G41">
+        <f t="shared" si="2"/>
+        <v>151710</v>
+      </c>
+      <c r="H41" s="6">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="I41">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="6">
+        <v>400</v>
+      </c>
+      <c r="B42">
+        <f t="shared" si="0"/>
+        <v>79800</v>
+      </c>
+      <c r="C42" s="6">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="D42">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F42" s="6">
+        <v>400</v>
+      </c>
+      <c r="G42">
+        <f t="shared" si="2"/>
+        <v>159600</v>
+      </c>
+      <c r="H42" s="6">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="I42">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="6">
+        <v>410</v>
+      </c>
+      <c r="B43">
+        <f t="shared" si="0"/>
+        <v>83845</v>
+      </c>
+      <c r="C43" s="6">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="D43">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F43" s="6">
+        <v>410</v>
+      </c>
+      <c r="G43">
+        <f t="shared" si="2"/>
+        <v>167690</v>
+      </c>
+      <c r="H43" s="6">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="I43">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="6">
+        <v>420</v>
+      </c>
+      <c r="B44">
+        <f t="shared" si="0"/>
+        <v>87990</v>
+      </c>
+      <c r="C44" s="6">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="D44">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F44" s="6">
+        <v>420</v>
+      </c>
+      <c r="G44">
+        <f t="shared" si="2"/>
+        <v>175980</v>
+      </c>
+      <c r="H44" s="6">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="I44">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="6">
+        <v>430</v>
+      </c>
+      <c r="B45">
+        <f t="shared" si="0"/>
+        <v>92235</v>
+      </c>
+      <c r="C45" s="6">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="D45">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="F45" s="6">
+        <v>430</v>
+      </c>
+      <c r="G45">
+        <f t="shared" si="2"/>
+        <v>184470</v>
+      </c>
+      <c r="H45" s="6">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="I45">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="6">
+        <v>440</v>
+      </c>
+      <c r="B46">
+        <f t="shared" si="0"/>
+        <v>96580</v>
+      </c>
+      <c r="C46" s="6">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="D46">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="F46" s="6">
+        <v>440</v>
+      </c>
+      <c r="G46">
+        <f t="shared" si="2"/>
+        <v>193160</v>
+      </c>
+      <c r="H46" s="6">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="I46">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" s="6">
+        <v>450</v>
+      </c>
+      <c r="B47">
+        <f t="shared" si="0"/>
+        <v>101025</v>
+      </c>
+      <c r="C47" s="6">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="D47">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="F47" s="6">
+        <v>450</v>
+      </c>
+      <c r="G47">
+        <f t="shared" si="2"/>
+        <v>202050</v>
+      </c>
+      <c r="H47" s="6">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="I47">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="6">
+        <v>460</v>
+      </c>
+      <c r="B48">
+        <f t="shared" si="0"/>
+        <v>105570</v>
+      </c>
+      <c r="C48" s="6">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="D48">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F48" s="6">
+        <v>460</v>
+      </c>
+      <c r="G48">
+        <f t="shared" si="2"/>
+        <v>211140</v>
+      </c>
+      <c r="H48" s="6">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="I48">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" s="6">
+        <v>470</v>
+      </c>
+      <c r="B49">
+        <f t="shared" si="0"/>
+        <v>110215</v>
+      </c>
+      <c r="C49" s="6">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="D49">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F49" s="6">
+        <v>470</v>
+      </c>
+      <c r="G49">
+        <f t="shared" si="2"/>
+        <v>220430</v>
+      </c>
+      <c r="H49" s="6">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="I49">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" s="6">
+        <v>480</v>
+      </c>
+      <c r="B50">
+        <f t="shared" si="0"/>
+        <v>114960</v>
+      </c>
+      <c r="C50" s="6">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="D50">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F50" s="6">
+        <v>480</v>
+      </c>
+      <c r="G50">
+        <f t="shared" si="2"/>
+        <v>229920</v>
+      </c>
+      <c r="H50" s="6">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="I50">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" s="6">
+        <v>490</v>
+      </c>
+      <c r="B51">
+        <f t="shared" si="0"/>
+        <v>119805</v>
+      </c>
+      <c r="C51" s="6">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="D51">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F51" s="6">
+        <v>490</v>
+      </c>
+      <c r="G51">
+        <f t="shared" si="2"/>
+        <v>239610</v>
+      </c>
+      <c r="H51" s="6">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="I51">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" s="6">
+        <v>500</v>
+      </c>
+      <c r="B52">
+        <f t="shared" si="0"/>
+        <v>124750</v>
+      </c>
+      <c r="C52" s="6">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="D52">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F52" s="6">
+        <v>500</v>
+      </c>
+      <c r="G52">
+        <f t="shared" si="2"/>
+        <v>249500</v>
+      </c>
+      <c r="H52" s="6">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="I52">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="F1:I1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>